<commit_message>
deux fonctions non complementaires
</commit_message>
<xml_diff>
--- a/AMouvementsData.xlsx
+++ b/AMouvementsData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mouvements Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -532,11 +533,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -748,29 +749,233 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3">
+        <v>17200</v>
+      </c>
+      <c r="D1" s="5">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3">
+        <v>22650</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3">
+        <v>14700</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3">
+        <v>21750</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3">
+        <v>15880</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3">
+        <v>25120</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3">
+        <v>22150</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3">
+        <v>22150</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3">
+        <v>15020</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25250</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3">
         <v>17200</v>
       </c>
       <c r="D11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3">
         <v>22650</v>
@@ -778,121 +983,115 @@
       <c r="D12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3">
-        <v>14700</v>
+        <v>15880</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3">
+        <v>25120</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3">
+        <v>22150</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
         <v>25</v>
       </c>
-      <c r="C14" s="3">
-        <v>21750</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3">
+        <v>15020</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
         <v>26</v>
       </c>
-      <c r="C15" s="3">
-        <v>15880</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="H15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3">
+        <v>25120</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
         <v>27</v>
       </c>
-      <c r="C16" s="3">
-        <v>25120</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="3">
-        <v>22150</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18">
-        <v>17</v>
-      </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3">
         <v>22150</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3">
         <v>15020</v>
@@ -900,13 +1099,17 @@
       <c r="D19" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
+      <c r="E19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3">
         <v>25250</v>
@@ -914,36 +1117,33 @@
       <c r="D20" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
+      <c r="E20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3">
         <v>17200</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="H21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3">
         <v>22650</v>
@@ -951,215 +1151,190 @@
       <c r="D22" s="5">
         <v>1</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="E22" s="3"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="3">
+        <v>14700</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="3">
+        <v>21750</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
         <v>34</v>
       </c>
-      <c r="C23" s="3">
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3">
         <v>15880</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="3">
-        <v>25120</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="3">
-        <v>22150</v>
-      </c>
       <c r="D25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="3">
-        <v>15020</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="3">
-        <v>25120</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="3">
-        <v>22150</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="3">
-        <v>15020</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="3">
-        <v>25250</v>
-      </c>
-      <c r="D30" s="5">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="3">
-        <v>17200</v>
-      </c>
-      <c r="D31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="3">
-        <v>22650</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="3">
-        <v>14700</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="3">
-        <v>21750</v>
-      </c>
-      <c r="D34" s="5">
         <v>0</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="3">
-        <v>15880</v>
-      </c>
-      <c r="D35" s="5">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="E25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="C26" s="3"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="3"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="C27" s="3"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="3"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="C28" s="3"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="3"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="C29" s="3"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="3"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="C30" s="3"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="3"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="C31" s="3"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="3"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="C32" s="3"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="3"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="3"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="3"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="C34" s="3"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="3"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="C35" s="3"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="3"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="3"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="3"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="C37" s="3"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="3"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="3:7">
+      <c r="C38" s="3"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="3"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="3:7">
+      <c r="C39" s="3"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="3"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="3:7">
+      <c r="C40" s="3"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="3"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="C41" s="3"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="3"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="C42" s="3"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="3"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="C43" s="3"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="3"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="3:7">
+      <c r="C44" s="3"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="3"/>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="C45" s="3"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="3"/>
+      <c r="G45" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>